<commit_message>
Delete clase Espia y Add tests comunicadorEspias y fix comEspias y excel
</commit_message>
<xml_diff>
--- a/src/lista_de_espias/lista-de-espias.xlsx
+++ b/src/lista_de_espias/lista-de-espias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25216"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3269A360-0597-4E0F-970F-B43F1BECC3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,47 +27,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Compañero</t>
-  </si>
-  <si>
-    <t>Probalidad</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
     <t>Ivan</t>
   </si>
   <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>Ruben</t>
   </si>
   <si>
     <t>William</t>
   </si>
   <si>
-    <t>0.35</t>
-  </si>
-  <si>
     <t>Rodolfo</t>
   </si>
   <si>
-    <t>0.45</t>
+    <t>Pepe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,8 +91,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,85 +407,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add carga de comunicaciones desde excel y casos de test, Add package tests
</commit_message>
<xml_diff>
--- a/src/lista_de_espias/lista-de-espias.xlsx
+++ b/src/lista_de_espias/lista-de-espias.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
@@ -48,22 +48,35 @@
   </si>
   <si>
     <t>Pepe</t>
+  </si>
+  <si>
+    <t>Compañero</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>Probabilidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,55 +421,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" s="1"/>
-    </row>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Add obtener agmComunicador y caso de test, add mas espias y relaciones
</commit_message>
<xml_diff>
--- a/src/lista_de_espias/lista-de-espias.xlsx
+++ b/src/lista_de_espias/lista-de-espias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18855" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Nombre</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>Probabilidad</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>Julieta</t>
+  </si>
+  <si>
+    <t>Mabel</t>
+  </si>
+  <si>
+    <t>Gabriela</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Candela</t>
+  </si>
+  <si>
+    <t>0.8</t>
   </si>
 </sst>
 </file>
@@ -421,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,8 +539,94 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>